<commit_message>
First attempt to production
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\renato\dev\o2o\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145868CF-A7E2-4D77-8780-FA6CA023030C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD68DE36-257D-4BC6-B712-707CA7923633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{254CB624-1491-43DA-A19E-C9BA6C6907F9}"/>
   </bookViews>
@@ -105,7 +105,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,13 +141,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,12 +466,13 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
@@ -524,6 +538,9 @@
       <c r="E2" t="b">
         <v>1</v>
       </c>
+      <c r="G2" s="1">
+        <v>150</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -540,6 +557,9 @@
       </c>
       <c r="E3" t="b">
         <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>75.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>